<commit_message>
Integrate web server and database for enhanced solver visualization and logging
Add web server and database integration for real-time visualization, logging, and data persistence of the Branch-and-Price solver.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9bcbd8ab-d31a-4685-81ce-32eaa55d4232
Replit-Commit-Checkpoint-Type: full_checkpoint
</commit_message>
<xml_diff>
--- a/output/algorithm_comparison.xlsx
+++ b/output/algorithm_comparison.xlsx
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02304267883300781</v>
+        <v>0.2615716457366943</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.2606146335601807</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>104.8999229583518</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>

</xml_diff>